<commit_message>
Fix dog vaccination rate parameter (alpha_d1: 0.001 -> 0.01)
</commit_message>
<xml_diff>
--- a/data/model_parameters.xlsx
+++ b/data/model_parameters.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cdc-my.sharepoint.com/personal/mfl3_cdc_gov/Documents/Rabies/RabioesEcon-Python/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravik\OneDrive\Documents\My-Projects\RabiesEcon-in-Python\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="11_F25DC773A252ABDACC1048DB71585A4C5BDE5913" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{722903C9-7E65-4D70-B289-1CFD6B06E202}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8024095D-C889-4E93-B1A7-2AE0D2F5C31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Type</t>
   </si>
@@ -126,6 +129,21 @@
   </si>
   <si>
     <t>Values_extra</t>
+  </si>
+  <si>
+    <t>Free_roaming_dog_population</t>
+  </si>
+  <si>
+    <t>Calculated</t>
+  </si>
+  <si>
+    <t>Humans_per_km2</t>
+  </si>
+  <si>
+    <t>Free_roaming_dogs_per_km2</t>
+  </si>
+  <si>
+    <t>Humans per km2</t>
   </si>
 </sst>
 </file>
@@ -178,6 +196,69 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Log"/>
+      <sheetName val="Title"/>
+      <sheetName val="Instructions"/>
+      <sheetName val="Define_program"/>
+      <sheetName val="Malawi TZs"/>
+      <sheetName val="Vax_cover"/>
+      <sheetName val="Probabilities"/>
+      <sheetName val="DALY"/>
+      <sheetName val="Vaccination_Cost"/>
+      <sheetName val="PEP_and_other_Costs"/>
+      <sheetName val="Summary"/>
+      <sheetName val="Other_Inputs"/>
+      <sheetName val="data"/>
+      <sheetName val="data_discounted"/>
+      <sheetName val="initial_run"/>
+      <sheetName val="no_vaccination"/>
+      <sheetName val="annual_vax"/>
+      <sheetName val="option2"/>
+      <sheetName val="Other_Inputs_Calculations"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3">
+        <row r="14">
+          <cell r="B14" t="str">
+            <v>FREE ROAMING Dog population</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15" t="str">
+            <v>FREE ROAMING Dogs per km2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,22 +524,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="53.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="28.44140625" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="4" max="4" width="53.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +556,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -492,7 +573,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -500,7 +581,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>14100000</v>
+        <v>13125164</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -509,7 +590,7 @@
         <v>11172223</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -526,7 +607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -543,7 +624,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -551,7 +632,7 @@
         <v>12</v>
       </c>
       <c r="C6">
-        <v>15</v>
+        <v>15.6</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
@@ -560,7 +641,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -577,7 +658,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -594,89 +675,134 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>1.5</v>
+        <v>0.03</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10">
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11">
-        <v>0.01</v>
+        <v>0.17</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12">
-        <v>0.17</v>
+        <v>5.1E-5</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E12">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13">
-        <v>5.1E-5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13">
         <v>1.5999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14">
+        <f>C3/C2</f>
+        <v>730.79977728285076</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <f>C3/C6</f>
+        <v>841356.66666666663</v>
+      </c>
+      <c r="D15" t="str">
+        <f>[1]Define_program!B14</f>
+        <v>FREE ROAMING Dog population</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16">
+        <f>C15/C2</f>
+        <v>46.846139569413509</v>
+      </c>
+      <c r="D16" t="str">
+        <f>[1]Define_program!B15</f>
+        <v>FREE ROAMING Dogs per km2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <f>0.34*LN(C16)</f>
+        <v>1.3079353258667055</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean up repository for public release
- Move development files to archive/ (excluded from tracking)
- Remove empty folders and unused directories
- Update .gitignore to exclude archive files
- Rename initial_run.py to notebooks_initial_run.py for clarity
- Keep only essential files: app/, data/, config/, docs/
- Clean README for public repository
</commit_message>
<xml_diff>
--- a/data/model_parameters.xlsx
+++ b/data/model_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravik\OneDrive\Documents\My-Projects\RabiesEcon-in-Python\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7246A1ED-539D-4E41-92A1-045F89D113E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52972B82-EAF7-476A-85B4-0D8342C02101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17110" yWindow="-2775" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2148,17 +2148,28 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
@@ -2168,6 +2179,84 @@
       <alignment horizontal="right" vertical="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="5" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="5" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="5" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2264,93 +2353,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="5" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="5" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="5" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2363,8 +2365,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2875,9 +2875,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:D23"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2910,43 +2910,43 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="217" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="217" t="s">
+    <row r="2" spans="1:6" s="154" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A2" s="154" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="217" t="s">
+      <c r="B2" s="154" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="217" t="s">
+      <c r="C2" s="154" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="218">
+      <c r="D2" s="155">
         <v>54560</v>
       </c>
-      <c r="E2" s="217" t="s">
+      <c r="E2" s="154" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="217">
+      <c r="F2" s="154">
         <v>17960</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="217" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A3" s="217" t="s">
+    <row r="3" spans="1:6" s="154" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A3" s="154" t="s">
         <v>147</v>
       </c>
-      <c r="B3" s="217" t="s">
+      <c r="B3" s="154" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="217" t="s">
+      <c r="C3" s="154" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="218">
+      <c r="D3" s="155">
         <v>41136000</v>
       </c>
-      <c r="E3" s="217" t="s">
+      <c r="E3" s="154" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="217">
+      <c r="F3" s="154">
         <v>13125164</v>
       </c>
     </row>
@@ -2990,23 +2990,23 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="217" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A6" s="217" t="s">
+    <row r="6" spans="1:6" s="154" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A6" s="154" t="s">
         <v>147</v>
       </c>
-      <c r="B6" s="217" t="s">
+      <c r="B6" s="154" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="217" t="s">
+      <c r="C6" s="154" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="217">
+      <c r="D6" s="154">
         <v>13</v>
       </c>
-      <c r="E6" s="217" t="s">
+      <c r="E6" s="154" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="217">
+      <c r="F6" s="154">
         <v>15.6</v>
       </c>
     </row>
@@ -3345,6 +3345,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3353,7 +3354,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -3491,14 +3492,14 @@
       <c r="F3" s="75"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.75">
-      <c r="A4" s="154" t="s">
+      <c r="A4" s="156" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="154"/>
-      <c r="C4" s="154"/>
-      <c r="D4" s="154"/>
-      <c r="E4" s="154"/>
-      <c r="F4" s="154"/>
+      <c r="B4" s="156"/>
+      <c r="C4" s="156"/>
+      <c r="D4" s="156"/>
+      <c r="E4" s="156"/>
+      <c r="F4" s="156"/>
     </row>
     <row r="5" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A5" s="81"/>
@@ -3915,16 +3916,16 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="194" t="s">
+      <c r="H5" s="174" t="s">
         <v>54</v>
       </c>
-      <c r="I5" s="195"/>
-      <c r="J5" s="196">
+      <c r="I5" s="175"/>
+      <c r="J5" s="176">
         <v>0.1</v>
       </c>
-      <c r="K5" s="197"/>
-      <c r="L5" s="198"/>
-      <c r="M5" s="199"/>
+      <c r="K5" s="177"/>
+      <c r="L5" s="178"/>
+      <c r="M5" s="179"/>
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
       <c r="P5" s="11"/>
@@ -3973,30 +3974,30 @@
         <v>59</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="H7" s="200" t="s">
+      <c r="H7" s="180" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="201"/>
-      <c r="J7" s="202" t="s">
+      <c r="I7" s="181"/>
+      <c r="J7" s="182" t="s">
         <v>56</v>
       </c>
-      <c r="K7" s="202"/>
-      <c r="L7" s="203" t="s">
+      <c r="K7" s="182"/>
+      <c r="L7" s="157" t="s">
         <v>61</v>
       </c>
-      <c r="M7" s="203"/>
-      <c r="N7" s="203" t="s">
+      <c r="M7" s="157"/>
+      <c r="N7" s="157" t="s">
         <v>62</v>
       </c>
-      <c r="O7" s="203"/>
-      <c r="P7" s="204"/>
+      <c r="O7" s="157"/>
+      <c r="P7" s="158"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
     </row>
     <row r="8" spans="1:20" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
-      <c r="A8" s="187" t="s">
+      <c r="A8" s="213" t="s">
         <v>63</v>
       </c>
       <c r="B8" s="17" t="s">
@@ -4016,32 +4017,32 @@
         <v>46046</v>
       </c>
       <c r="G8" s="6"/>
-      <c r="H8" s="189" t="s">
+      <c r="H8" s="172" t="s">
         <v>65</v>
       </c>
-      <c r="I8" s="190"/>
-      <c r="J8" s="191">
+      <c r="I8" s="173"/>
+      <c r="J8" s="159">
         <f>B5</f>
         <v>656500</v>
       </c>
-      <c r="K8" s="192"/>
-      <c r="L8" s="193">
+      <c r="K8" s="160"/>
+      <c r="L8" s="161">
         <v>0.53</v>
       </c>
-      <c r="M8" s="193"/>
-      <c r="N8" s="158">
+      <c r="M8" s="161"/>
+      <c r="N8" s="162">
         <f>L8*J8</f>
         <v>347945</v>
       </c>
-      <c r="O8" s="158"/>
-      <c r="P8" s="159"/>
+      <c r="O8" s="162"/>
+      <c r="P8" s="163"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.75">
-      <c r="A9" s="173"/>
+      <c r="A9" s="199"/>
       <c r="B9" s="18" t="s">
         <v>66</v>
       </c>
@@ -4059,32 +4060,32 @@
         <v>21164</v>
       </c>
       <c r="G9" s="6"/>
-      <c r="H9" s="189" t="s">
+      <c r="H9" s="172" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="190"/>
-      <c r="J9" s="191">
+      <c r="I9" s="173"/>
+      <c r="J9" s="159">
         <f>B5</f>
         <v>656500</v>
       </c>
-      <c r="K9" s="192"/>
-      <c r="L9" s="193">
+      <c r="K9" s="160"/>
+      <c r="L9" s="161">
         <v>0.1</v>
       </c>
-      <c r="M9" s="193"/>
-      <c r="N9" s="158">
+      <c r="M9" s="161"/>
+      <c r="N9" s="162">
         <f>L9*J9</f>
         <v>65650</v>
       </c>
-      <c r="O9" s="158"/>
-      <c r="P9" s="159"/>
+      <c r="O9" s="162"/>
+      <c r="P9" s="163"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.75">
-      <c r="A10" s="173"/>
+      <c r="A10" s="199"/>
       <c r="B10" s="18" t="s">
         <v>68</v>
       </c>
@@ -4102,32 +4103,32 @@
         <v>66466.399999999994</v>
       </c>
       <c r="G10" s="6"/>
-      <c r="H10" s="211" t="s">
+      <c r="H10" s="170" t="s">
         <v>69</v>
       </c>
-      <c r="I10" s="212"/>
-      <c r="J10" s="191">
+      <c r="I10" s="171"/>
+      <c r="J10" s="159">
         <f>B5</f>
         <v>656500</v>
       </c>
-      <c r="K10" s="192"/>
-      <c r="L10" s="193">
+      <c r="K10" s="160"/>
+      <c r="L10" s="161">
         <v>0.05</v>
       </c>
-      <c r="M10" s="193"/>
-      <c r="N10" s="158">
+      <c r="M10" s="161"/>
+      <c r="N10" s="162">
         <f>L10*J10</f>
         <v>32825</v>
       </c>
-      <c r="O10" s="158"/>
-      <c r="P10" s="159"/>
+      <c r="O10" s="162"/>
+      <c r="P10" s="163"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="63"/>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.75">
-      <c r="A11" s="173"/>
+      <c r="A11" s="199"/>
       <c r="B11" s="18" t="s">
         <v>70</v>
       </c>
@@ -4145,33 +4146,33 @@
         <v>33233.199999999997</v>
       </c>
       <c r="G11" s="54"/>
-      <c r="H11" s="205" t="s">
+      <c r="H11" s="164" t="s">
         <v>71</v>
       </c>
-      <c r="I11" s="206"/>
-      <c r="J11" s="207">
+      <c r="I11" s="165"/>
+      <c r="J11" s="166">
         <f>B5</f>
         <v>656500</v>
       </c>
-      <c r="K11" s="208"/>
-      <c r="L11" s="209">
+      <c r="K11" s="167"/>
+      <c r="L11" s="168">
         <f>0.01507*C29</f>
         <v>1.5965858897603692E-2</v>
       </c>
-      <c r="M11" s="210"/>
-      <c r="N11" s="158">
+      <c r="M11" s="169"/>
+      <c r="N11" s="162">
         <f>L11*J11</f>
         <v>10481.586366276824</v>
       </c>
-      <c r="O11" s="158"/>
-      <c r="P11" s="159"/>
+      <c r="O11" s="162"/>
+      <c r="P11" s="163"/>
       <c r="Q11" s="61"/>
       <c r="R11" s="64"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
     </row>
     <row r="12" spans="1:20" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A12" s="173"/>
+      <c r="A12" s="199"/>
       <c r="B12" s="18" t="s">
         <v>72</v>
       </c>
@@ -4189,27 +4190,27 @@
         <v>143000</v>
       </c>
       <c r="G12" s="6"/>
-      <c r="H12" s="160" t="s">
+      <c r="H12" s="186" t="s">
         <v>73</v>
       </c>
-      <c r="I12" s="161"/>
-      <c r="J12" s="161"/>
-      <c r="K12" s="161"/>
-      <c r="L12" s="161"/>
-      <c r="M12" s="162"/>
-      <c r="N12" s="163">
+      <c r="I12" s="187"/>
+      <c r="J12" s="187"/>
+      <c r="K12" s="187"/>
+      <c r="L12" s="187"/>
+      <c r="M12" s="188"/>
+      <c r="N12" s="189">
         <f>SUM(N8:P11)*(1+J5)</f>
         <v>502591.74500290456</v>
       </c>
-      <c r="O12" s="164"/>
-      <c r="P12" s="165"/>
+      <c r="O12" s="190"/>
+      <c r="P12" s="191"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="64"/>
       <c r="S12" s="65"/>
       <c r="T12" s="6"/>
     </row>
     <row r="13" spans="1:20" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A13" s="188"/>
+      <c r="A13" s="214"/>
       <c r="B13" s="19" t="s">
         <v>74</v>
       </c>
@@ -4260,20 +4261,20 @@
         <v>165880</v>
       </c>
       <c r="G14" s="6"/>
-      <c r="H14" s="166" t="s">
+      <c r="H14" s="192" t="s">
         <v>76</v>
       </c>
-      <c r="I14" s="167"/>
-      <c r="J14" s="167"/>
-      <c r="K14" s="167"/>
-      <c r="L14" s="167"/>
-      <c r="M14" s="168"/>
-      <c r="N14" s="169">
+      <c r="I14" s="193"/>
+      <c r="J14" s="193"/>
+      <c r="K14" s="193"/>
+      <c r="L14" s="193"/>
+      <c r="M14" s="194"/>
+      <c r="N14" s="195">
         <f>SUM(L8:M11)*(1+J5)</f>
         <v>0.76556244478736424</v>
       </c>
-      <c r="O14" s="170"/>
-      <c r="P14" s="171"/>
+      <c r="O14" s="196"/>
+      <c r="P14" s="197"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
       <c r="S14" s="66"/>
@@ -4313,7 +4314,7 @@
       <c r="T15" s="6"/>
     </row>
     <row r="16" spans="1:20" ht="16.25" thickTop="1" x14ac:dyDescent="0.75">
-      <c r="A16" s="172" t="s">
+      <c r="A16" s="198" t="s">
         <v>78</v>
       </c>
       <c r="B16" s="17" t="s">
@@ -4333,27 +4334,27 @@
         <v>60060</v>
       </c>
       <c r="G16" s="6"/>
-      <c r="H16" s="175" t="s">
+      <c r="H16" s="201" t="s">
         <v>80</v>
       </c>
-      <c r="I16" s="176"/>
-      <c r="J16" s="176"/>
-      <c r="K16" s="176"/>
-      <c r="L16" s="176"/>
-      <c r="M16" s="177"/>
-      <c r="N16" s="178">
+      <c r="I16" s="202"/>
+      <c r="J16" s="202"/>
+      <c r="K16" s="202"/>
+      <c r="L16" s="202"/>
+      <c r="M16" s="203"/>
+      <c r="N16" s="204">
         <f>N14+(F21/B5)</f>
         <v>2.4508169763943712</v>
       </c>
-      <c r="O16" s="179"/>
-      <c r="P16" s="180"/>
+      <c r="O16" s="205"/>
+      <c r="P16" s="206"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
     </row>
     <row r="17" spans="1:20" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A17" s="173"/>
+      <c r="A17" s="199"/>
       <c r="B17" s="18" t="s">
         <v>81</v>
       </c>
@@ -4371,29 +4372,29 @@
         <v>22880</v>
       </c>
       <c r="G17" s="6"/>
-      <c r="H17" s="184" t="s">
+      <c r="H17" s="210" t="s">
         <v>82</v>
       </c>
-      <c r="I17" s="185"/>
-      <c r="J17" s="186">
+      <c r="I17" s="211"/>
+      <c r="J17" s="212">
         <f>B5</f>
         <v>656500</v>
       </c>
-      <c r="K17" s="185"/>
+      <c r="K17" s="211"/>
       <c r="L17" s="58" t="s">
         <v>83</v>
       </c>
       <c r="M17" s="59"/>
-      <c r="N17" s="181"/>
-      <c r="O17" s="182"/>
-      <c r="P17" s="183"/>
+      <c r="N17" s="207"/>
+      <c r="O17" s="208"/>
+      <c r="P17" s="209"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
     </row>
     <row r="18" spans="1:20" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A18" s="174"/>
+      <c r="A18" s="200"/>
       <c r="B18" s="22" t="s">
         <v>84</v>
       </c>
@@ -4426,7 +4427,7 @@
       <c r="T18" s="6"/>
     </row>
     <row r="19" spans="1:20" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
-      <c r="A19" s="155" t="s">
+      <c r="A19" s="183" t="s">
         <v>85</v>
       </c>
       <c r="B19" s="23" t="s">
@@ -4461,7 +4462,7 @@
       <c r="T19" s="6"/>
     </row>
     <row r="20" spans="1:20" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A20" s="156"/>
+      <c r="A20" s="184"/>
       <c r="B20" s="24" t="s">
         <v>87</v>
       </c>
@@ -4479,19 +4480,19 @@
         <v>0</v>
       </c>
       <c r="G20" s="6"/>
-      <c r="H20" s="157"/>
-      <c r="I20" s="157"/>
-      <c r="J20" s="157"/>
-      <c r="K20" s="157"/>
-      <c r="L20" s="157"/>
-      <c r="M20" s="157"/>
-      <c r="N20" s="157"/>
-      <c r="O20" s="157"/>
-      <c r="P20" s="157"/>
-      <c r="Q20" s="157"/>
-      <c r="R20" s="157"/>
-      <c r="S20" s="157"/>
-      <c r="T20" s="157"/>
+      <c r="H20" s="185"/>
+      <c r="I20" s="185"/>
+      <c r="J20" s="185"/>
+      <c r="K20" s="185"/>
+      <c r="L20" s="185"/>
+      <c r="M20" s="185"/>
+      <c r="N20" s="185"/>
+      <c r="O20" s="185"/>
+      <c r="P20" s="185"/>
+      <c r="Q20" s="185"/>
+      <c r="R20" s="185"/>
+      <c r="S20" s="185"/>
+      <c r="T20" s="185"/>
     </row>
     <row r="21" spans="1:20" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A21" s="9" t="s">
@@ -4506,19 +4507,19 @@
         <v>1106369.6000000001</v>
       </c>
       <c r="G21" s="6"/>
-      <c r="H21" s="157"/>
-      <c r="I21" s="157"/>
-      <c r="J21" s="157"/>
-      <c r="K21" s="157"/>
-      <c r="L21" s="157"/>
-      <c r="M21" s="157"/>
-      <c r="N21" s="157"/>
-      <c r="O21" s="157"/>
-      <c r="P21" s="157"/>
-      <c r="Q21" s="157"/>
-      <c r="R21" s="157"/>
-      <c r="S21" s="157"/>
-      <c r="T21" s="157"/>
+      <c r="H21" s="185"/>
+      <c r="I21" s="185"/>
+      <c r="J21" s="185"/>
+      <c r="K21" s="185"/>
+      <c r="L21" s="185"/>
+      <c r="M21" s="185"/>
+      <c r="N21" s="185"/>
+      <c r="O21" s="185"/>
+      <c r="P21" s="185"/>
+      <c r="Q21" s="185"/>
+      <c r="R21" s="185"/>
+      <c r="S21" s="185"/>
+      <c r="T21" s="185"/>
     </row>
     <row r="22" spans="1:20" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
       <c r="A22" s="10" t="s">
@@ -4738,24 +4739,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="H20:T21"/>
     <mergeCell ref="N11:P11"/>
@@ -4772,6 +4755,24 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:M8"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:P9"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Costs per dog vaccinated" prompt="Enter the estimated cost per dog vaccinated.  Costs are presented in USD, therefore user will need to convert into their local currency. " sqref="B5" xr:uid="{69D90B4D-BC64-4C0C-9B68-3F349EA33EB4}"/>
@@ -4789,8 +4790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F108F679-BD74-4A2A-8C34-09F8E58E32B0}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -4831,11 +4832,11 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3" s="12"/>
-      <c r="B3" s="213" t="str">
+      <c r="B3" s="215" t="str">
         <f>"Parameters for Disability Adjusted Life Years (DALY (YLL)) estimates at a "&amp;TEXT(discount_rate,"0%")&amp;" discount rate, r"</f>
         <v>Parameters for Disability Adjusted Life Years (DALY (YLL)) estimates at a 3% discount rate, r</v>
       </c>
-      <c r="C3" s="214"/>
+      <c r="C3" s="216"/>
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
@@ -4995,14 +4996,14 @@
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="215" t="s">
+      <c r="E12" s="217" t="s">
         <v>132</v>
       </c>
-      <c r="F12" s="215"/>
-      <c r="G12" s="215"/>
-      <c r="H12" s="215"/>
-      <c r="I12" s="215"/>
-      <c r="J12" s="215"/>
+      <c r="F12" s="217"/>
+      <c r="G12" s="217"/>
+      <c r="H12" s="217"/>
+      <c r="I12" s="217"/>
+      <c r="J12" s="217"/>
       <c r="K12" s="12"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.75">
@@ -5012,12 +5013,12 @@
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="215"/>
-      <c r="F13" s="215"/>
-      <c r="G13" s="215"/>
-      <c r="H13" s="215"/>
-      <c r="I13" s="215"/>
-      <c r="J13" s="215"/>
+      <c r="E13" s="217"/>
+      <c r="F13" s="217"/>
+      <c r="G13" s="217"/>
+      <c r="H13" s="217"/>
+      <c r="I13" s="217"/>
+      <c r="J13" s="217"/>
       <c r="K13" s="12"/>
     </row>
     <row r="14" spans="1:11" ht="101.5" x14ac:dyDescent="0.75">
@@ -5163,13 +5164,13 @@
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
-      <c r="E20" s="216" t="s">
+      <c r="E20" s="218" t="s">
         <v>144</v>
       </c>
-      <c r="F20" s="216"/>
-      <c r="G20" s="216"/>
-      <c r="H20" s="216"/>
-      <c r="I20" s="216"/>
+      <c r="F20" s="218"/>
+      <c r="G20" s="218"/>
+      <c r="H20" s="218"/>
+      <c r="I20" s="218"/>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
     </row>

</xml_diff>